<commit_message>
Working Fine : Real time Conversiation
</commit_message>
<xml_diff>
--- a/letsDiscuss/documentation/serverAPIs.xlsx
+++ b/letsDiscuss/documentation/serverAPIs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\FullStackProject\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Html_CSS\letsDiscuss\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1100B928-BED9-4D23-9425-8BDA622C950E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D3DCFE-B5FA-42CD-BB7D-1F3E5223EF94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2228,7 +2228,7 @@
   <dimension ref="A1:R52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3924,7 +3924,7 @@
       <c r="A39" s="15">
         <v>37</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="16" t="s">
         <v>298</v>
       </c>
       <c r="C39" s="14"/>
@@ -3968,7 +3968,7 @@
       <c r="A40" s="15">
         <v>38</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="16" t="s">
         <v>304</v>
       </c>
       <c r="C40" s="14"/>
@@ -4012,7 +4012,7 @@
       <c r="A41" s="15">
         <v>39</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="16" t="s">
         <v>310</v>
       </c>
       <c r="C41" s="14"/>
@@ -4056,7 +4056,7 @@
       <c r="A42" s="15">
         <v>40</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="16" t="s">
         <v>316</v>
       </c>
       <c r="C42" s="14"/>
@@ -8940,21 +8940,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A855378936633F46935DE081F3F0A723" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fb8377a16f57469f31fda63402737be">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a5a807ddb17e97ebd5eac858e2e697fd" ns3:_="">
     <xsd:import namespace="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
@@ -9156,31 +9141,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A8016DE-DC46-404F-9AC8-AB31FBBA1BB2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9196,4 +9172,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7DF4A1F3-27F5-4026-9F7B-EA2EEA754838}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{88BC72A4-2999-4A2E-B325-3F14F9A9DFDC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="0e1bb11d-1fe8-4e80-a80d-c671e8cd2a50"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>